<commit_message>
Changes to testing out different cost sensitive classifiers
</commit_message>
<xml_diff>
--- a/data/labeled_claims/consumer_price_index_claims.xlsx
+++ b/data/labeled_claims/consumer_price_index_claims.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="356">
   <si>
     <t>N</t>
   </si>
@@ -1092,6 +1092,9 @@
   </si>
   <si>
     <t>alias</t>
+  </si>
+  <si>
+    <t>sentence</t>
   </si>
 </sst>
 </file>
@@ -1488,7 +1491,7 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1497,6 +1500,9 @@
       <c r="A1" t="s">
         <v>350</v>
       </c>
+      <c r="C1" t="s">
+        <v>355</v>
+      </c>
       <c r="D1" t="s">
         <v>353</v>
       </c>

</xml_diff>

<commit_message>
Deleting old files from repo
</commit_message>
<xml_diff>
--- a/data/labeled_claims/consumer_price_index_claims.xlsx
+++ b/data/labeled_claims/consumer_price_index_claims.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="357">
   <si>
     <t>N</t>
   </si>
@@ -1095,6 +1095,9 @@
   </si>
   <si>
     <t>sentence</t>
+  </si>
+  <si>
+    <t>dep</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1494,7 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1512,6 +1515,9 @@
       <c r="G1" t="s">
         <v>351</v>
       </c>
+      <c r="I1" t="s">
+        <v>356</v>
+      </c>
       <c r="J1" t="s">
         <v>352</v>
       </c>

</xml_diff>